<commit_message>
Update Generated TOR gamelog
</commit_message>
<xml_diff>
--- a/Data/TOR_PlayerReplacement_V2.xlsx
+++ b/Data/TOR_PlayerReplacement_V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cindy\Big Data\GitHub\Capstone\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\McMaster\DAT205\Capstone\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A861FACD-26E6-4767-A218-66B6022BBF13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E83B4B5-1B2D-4EA2-B073-19530E732738}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{42968B75-5DCE-4E0E-9A9A-B8A53223C097}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{42968B75-5DCE-4E0E-9A9A-B8A53223C097}"/>
   </bookViews>
   <sheets>
     <sheet name="TOR" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="94">
   <si>
     <t>PLAYER_ID</t>
   </si>
@@ -729,18 +729,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615D710C-326D-4A13-89C8-C56D828218D6}">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="28" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="28" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -826,7 +826,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1629044</v>
       </c>
@@ -912,7 +912,7 @@
         <v>37.431452141608389</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1627775</v>
       </c>
@@ -998,7 +998,7 @@
         <v>7.6624284150229727</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1626169</v>
       </c>
@@ -1084,8 +1084,8 @@
         <v>13.298704081225454</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1093,331 +1093,257 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427216FC-37D8-411D-BA13-86BA098230C8}">
-  <dimension ref="A1:AM4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="25" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1626166</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3">
+        <v>22.89479166666667</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4.125</v>
+      </c>
+      <c r="E2" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.49225000000000002</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.875</v>
+      </c>
+      <c r="H2" s="3">
+        <v>3.625</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.208375</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N2" s="3">
+        <v>3.375</v>
+      </c>
+      <c r="O2" s="3">
+        <v>3.875</v>
+      </c>
+      <c r="P2" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1.375</v>
+      </c>
+      <c r="R2" s="3">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="S2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="U2" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="V2" s="3">
+        <v>1.125</v>
+      </c>
+      <c r="W2" s="3">
+        <v>10.875</v>
+      </c>
+      <c r="X2" s="3">
+        <v>11.125</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>8.6514443968468111</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>18.681443157183651</v>
+      </c>
+      <c r="AC2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>202732</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="3">
+        <v>24.616666666666671</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
         <v>2</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="K3" s="3">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="L3" s="3">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M3" s="3">
+        <v>3</v>
+      </c>
+      <c r="N3" s="3">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="O3" s="3">
         <v>7</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1626166</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1610612756</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="3">
-        <v>22.89479166666667</v>
-      </c>
-      <c r="L2" s="3">
-        <v>4.125</v>
-      </c>
-      <c r="M2" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.49225000000000002</v>
-      </c>
-      <c r="O2" s="3">
-        <v>1.875</v>
-      </c>
-      <c r="P2" s="3">
-        <v>3.625</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>0.51249999999999996</v>
-      </c>
-      <c r="R2" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="S2" s="3">
-        <v>0.875</v>
-      </c>
-      <c r="T2" s="3">
-        <v>0.208375</v>
-      </c>
-      <c r="U2" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="V2" s="3">
-        <v>3.375</v>
-      </c>
-      <c r="W2" s="3">
-        <v>3.875</v>
-      </c>
-      <c r="X2" s="3">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>1.375</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>1.125</v>
-      </c>
-      <c r="AE2" s="3">
-        <v>10.875</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>11.125</v>
-      </c>
-      <c r="AG2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK2" s="3">
-        <v>8.6514443968468111</v>
-      </c>
-      <c r="AL2" s="3">
-        <v>18.681443157183651</v>
-      </c>
-      <c r="AM2" s="3">
-        <v>1737145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="3">
-        <v>202732</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1610612742</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="3">
-        <v>24.616666666666671</v>
-      </c>
-      <c r="L3" s="3">
-        <v>3</v>
-      </c>
-      <c r="M3" s="3">
-        <v>6</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O3" s="3">
-        <v>0</v>
-      </c>
       <c r="P3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="3">
         <v>0</v>
@@ -1426,187 +1352,123 @@
         <v>2</v>
       </c>
       <c r="S3" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T3" s="3">
-        <v>0.66700000000000004</v>
+        <v>1</v>
       </c>
       <c r="U3" s="3">
         <v>3</v>
       </c>
       <c r="V3" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W3" s="3">
+        <v>8</v>
+      </c>
+      <c r="X3" s="3">
         <v>7</v>
       </c>
-      <c r="X3" s="3">
-        <v>0</v>
-      </c>
       <c r="Y3" s="3">
         <v>0</v>
       </c>
       <c r="Z3" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="3">
-        <v>0</v>
+        <v>9.8265895953757223</v>
       </c>
       <c r="AB3" s="3">
+        <v>18.135233581584288</v>
+      </c>
+      <c r="AC3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>203953</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="3">
+        <v>13.411111111111111</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.45183333333333331</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I4" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="O4" s="3">
+        <v>3.8333333333333335</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="U4" s="3">
         <v>1</v>
       </c>
-      <c r="AC3" s="3">
-        <v>3</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="3">
-        <v>8</v>
-      </c>
-      <c r="AF3" s="3">
-        <v>7</v>
-      </c>
-      <c r="AG3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK3" s="3">
-        <v>9.8265895953757223</v>
-      </c>
-      <c r="AL3" s="3">
-        <v>18.135233581584288</v>
-      </c>
-      <c r="AM3" s="3">
-        <v>1015696</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="3">
-        <v>203953</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1610612758</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="3">
-        <v>13.411111111111111</v>
-      </c>
-      <c r="L4" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="M4" s="3">
-        <v>6</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0.45183333333333331</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="R4" s="3">
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="S4" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="T4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="U4" s="3">
-        <v>1.1666666666666667</v>
-      </c>
       <c r="V4" s="3">
-        <v>2.6666666666666665</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="W4" s="3">
-        <v>3.8333333333333335</v>
+        <v>8.5</v>
       </c>
       <c r="X4" s="3">
-        <v>1.6666666666666667</v>
+        <v>6.5</v>
       </c>
       <c r="Y4" s="3">
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>0.16666666666666666</v>
+        <v>8.486380200761797</v>
       </c>
       <c r="AB4" s="3">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="AC4" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="AE4" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="AF4" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="AG4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK4" s="3">
-        <v>8.486380200761797</v>
-      </c>
-      <c r="AL4" s="3">
         <v>25.496540816205599</v>
       </c>
-      <c r="AM4" s="3">
-        <v>6500000</v>
-      </c>
+      <c r="AC4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1621,9 +1483,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1709,7 +1571,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1629044</v>
       </c>
@@ -1795,7 +1657,7 @@
         <v>37.431452141608389</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1627775</v>
       </c>
@@ -1881,7 +1743,7 @@
         <v>7.6624284150229727</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1626169</v>
       </c>
@@ -1967,7 +1829,7 @@
         <v>13.298704081225454</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1628449</v>
       </c>
@@ -2053,7 +1915,7 @@
         <v>17.426078158129052</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1626178</v>
       </c>
@@ -2152,12 +2014,12 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2276,7 +2138,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2395,7 +2257,7 @@
         <v>1737145</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2514,7 +2376,7 @@
         <v>1015696</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -2633,7 +2495,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2752,7 +2614,7 @@
         <v>79568</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -2871,7 +2733,7 @@
         <v>3477600</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>

</xml_diff>